<commit_message>
Update - added user import validation
</commit_message>
<xml_diff>
--- a/testemail.xlsx
+++ b/testemail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tttt</t>
   </si>
 </sst>
 </file>
@@ -128,20 +131,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,22 +275,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -291,10 +298,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -302,7 +309,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -310,11 +317,31 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="marlon@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="marlon@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>